<commit_message>
clean TODOs, corrected exporting consumption of template, got back the changes on min dist between maints. Edited official template to be more representative.
</commit_message>
<xml_diff>
--- a/data/template/official/template_in.xlsx
+++ b/data/template/official/template_in.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pchtsp\Documents\projects\optima\data\template\official\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AC1752-6851-4E04-8AA2-2527CFDE770B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64751AC-F2A4-41F7-9B30-26A568685479}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="623" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="623" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="maintenances" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="158">
   <si>
     <t>maint</t>
   </si>
@@ -499,9 +499,6 @@
     <t>mois</t>
   </si>
   <si>
-    <t>2015-05</t>
-  </si>
-  <si>
     <t>2019-01</t>
   </si>
   <si>
@@ -515,6 +512,15 @@
   </si>
   <si>
     <t>2019-04</t>
+  </si>
+  <si>
+    <t>2019-05</t>
+  </si>
+  <si>
+    <t>2019-06</t>
+  </si>
+  <si>
+    <t>2019-07</t>
   </si>
 </sst>
 </file>
@@ -3909,8 +3915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3948,7 +3954,7 @@
         <v>126</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3977,7 +3983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -4666,7 +4672,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08E48A67-3B38-4D8C-86F5-29032CA09188}">
   <dimension ref="A1:C241"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4689,7 +4697,7 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C2">
         <v>14</v>
@@ -4700,7 +4708,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C3">
         <v>14</v>
@@ -4711,7 +4719,7 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C4">
         <v>14</v>
@@ -4722,7 +4730,7 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C5">
         <v>14</v>
@@ -4733,7 +4741,7 @@
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C6">
         <v>14</v>
@@ -4744,7 +4752,7 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C7">
         <v>14</v>
@@ -4755,7 +4763,7 @@
         <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C8">
         <v>14</v>
@@ -4766,7 +4774,7 @@
         <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C9">
         <v>14</v>
@@ -4777,7 +4785,7 @@
         <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C10">
         <v>14</v>
@@ -4788,7 +4796,7 @@
         <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C11">
         <v>14</v>
@@ -4799,7 +4807,7 @@
         <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C12">
         <v>14</v>
@@ -4810,7 +4818,7 @@
         <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C13">
         <v>14</v>
@@ -4821,7 +4829,7 @@
         <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C14">
         <v>14</v>
@@ -4832,7 +4840,7 @@
         <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -4843,7 +4851,7 @@
         <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C16">
         <v>14</v>
@@ -4854,7 +4862,7 @@
         <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C17">
         <v>14</v>
@@ -4865,7 +4873,7 @@
         <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C18">
         <v>14</v>
@@ -4876,7 +4884,7 @@
         <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C19">
         <v>14</v>
@@ -4887,7 +4895,7 @@
         <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C20">
         <v>14</v>
@@ -4898,7 +4906,7 @@
         <v>64</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C21">
         <v>14</v>
@@ -4909,7 +4917,7 @@
         <v>65</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C22">
         <v>14</v>
@@ -4920,7 +4928,7 @@
         <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C23">
         <v>14</v>
@@ -4931,7 +4939,7 @@
         <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C24">
         <v>14</v>
@@ -4942,7 +4950,7 @@
         <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C25">
         <v>14</v>
@@ -4953,7 +4961,7 @@
         <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C26">
         <v>14</v>
@@ -4964,7 +4972,7 @@
         <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C27">
         <v>14</v>
@@ -4975,7 +4983,7 @@
         <v>75</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C28">
         <v>14</v>
@@ -4986,7 +4994,7 @@
         <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C29">
         <v>14</v>
@@ -4997,7 +5005,7 @@
         <v>77</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C30">
         <v>14</v>
@@ -5008,7 +5016,7 @@
         <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C31">
         <v>14</v>
@@ -5019,7 +5027,7 @@
         <v>80</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C32">
         <v>14</v>
@@ -5030,7 +5038,7 @@
         <v>81</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C33">
         <v>14</v>
@@ -5041,7 +5049,7 @@
         <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C34">
         <v>14</v>
@@ -5052,7 +5060,7 @@
         <v>84</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C35">
         <v>14</v>
@@ -5063,7 +5071,7 @@
         <v>86</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C36">
         <v>14</v>
@@ -5074,7 +5082,7 @@
         <v>87</v>
       </c>
       <c r="B37" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C37">
         <v>14</v>
@@ -5085,7 +5093,7 @@
         <v>88</v>
       </c>
       <c r="B38" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C38">
         <v>14</v>
@@ -5096,7 +5104,7 @@
         <v>90</v>
       </c>
       <c r="B39" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C39">
         <v>14</v>
@@ -5107,7 +5115,7 @@
         <v>92</v>
       </c>
       <c r="B40" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C40">
         <v>14</v>
@@ -5118,7 +5126,7 @@
         <v>93</v>
       </c>
       <c r="B41" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C41">
         <v>14</v>
@@ -5129,7 +5137,7 @@
         <v>94</v>
       </c>
       <c r="B42" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C42">
         <v>14</v>
@@ -5140,7 +5148,7 @@
         <v>96</v>
       </c>
       <c r="B43" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C43">
         <v>14</v>
@@ -5151,7 +5159,7 @@
         <v>97</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C44">
         <v>14</v>
@@ -5162,7 +5170,7 @@
         <v>98</v>
       </c>
       <c r="B45" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C45">
         <v>14</v>
@@ -5173,7 +5181,7 @@
         <v>100</v>
       </c>
       <c r="B46" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C46">
         <v>14</v>
@@ -5184,7 +5192,7 @@
         <v>101</v>
       </c>
       <c r="B47" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C47">
         <v>14</v>
@@ -5195,7 +5203,7 @@
         <v>103</v>
       </c>
       <c r="B48" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C48">
         <v>14</v>
@@ -5206,7 +5214,7 @@
         <v>105</v>
       </c>
       <c r="B49" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C49">
         <v>14</v>
@@ -5217,7 +5225,7 @@
         <v>106</v>
       </c>
       <c r="B50" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C50">
         <v>14</v>
@@ -5228,7 +5236,7 @@
         <v>109</v>
       </c>
       <c r="B51" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C51">
         <v>14</v>
@@ -5239,7 +5247,7 @@
         <v>110</v>
       </c>
       <c r="B52" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C52">
         <v>14</v>
@@ -5250,7 +5258,7 @@
         <v>111</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C53">
         <v>14</v>
@@ -5261,7 +5269,7 @@
         <v>112</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C54">
         <v>14</v>
@@ -5272,7 +5280,7 @@
         <v>113</v>
       </c>
       <c r="B55" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C55">
         <v>14</v>
@@ -5283,7 +5291,7 @@
         <v>114</v>
       </c>
       <c r="B56" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C56">
         <v>14</v>
@@ -5294,7 +5302,7 @@
         <v>115</v>
       </c>
       <c r="B57" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C57">
         <v>14</v>
@@ -5305,7 +5313,7 @@
         <v>116</v>
       </c>
       <c r="B58" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C58">
         <v>14</v>
@@ -5316,7 +5324,7 @@
         <v>117</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C59">
         <v>14</v>
@@ -5327,7 +5335,7 @@
         <v>119</v>
       </c>
       <c r="B60" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C60">
         <v>14</v>
@@ -5338,7 +5346,7 @@
         <v>121</v>
       </c>
       <c r="B61" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="C61">
         <v>14</v>
@@ -5349,7 +5357,7 @@
         <v>19</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C62">
         <v>18</v>
@@ -5360,7 +5368,7 @@
         <v>23</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C63">
         <v>18</v>
@@ -5371,7 +5379,7 @@
         <v>27</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C64">
         <v>18</v>
@@ -5382,7 +5390,7 @@
         <v>30</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C65">
         <v>18</v>
@@ -5393,7 +5401,7 @@
         <v>33</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C66">
         <v>18</v>
@@ -5404,7 +5412,7 @@
         <v>36</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C67">
         <v>18</v>
@@ -5415,7 +5423,7 @@
         <v>38</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C68">
         <v>18</v>
@@ -5426,7 +5434,7 @@
         <v>41</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C69">
         <v>18</v>
@@ -5437,7 +5445,7 @@
         <v>44</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C70">
         <v>18</v>
@@ -5448,7 +5456,7 @@
         <v>46</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C71">
         <v>18</v>
@@ -5459,7 +5467,7 @@
         <v>48</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C72">
         <v>18</v>
@@ -5470,7 +5478,7 @@
         <v>49</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C73">
         <v>18</v>
@@ -5481,7 +5489,7 @@
         <v>51</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C74">
         <v>18</v>
@@ -5492,7 +5500,7 @@
         <v>53</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C75">
         <v>18</v>
@@ -5503,7 +5511,7 @@
         <v>54</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C76">
         <v>18</v>
@@ -5514,7 +5522,7 @@
         <v>57</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C77">
         <v>18</v>
@@ -5525,7 +5533,7 @@
         <v>59</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C78">
         <v>18</v>
@@ -5536,7 +5544,7 @@
         <v>61</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C79">
         <v>18</v>
@@ -5547,7 +5555,7 @@
         <v>62</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C80">
         <v>18</v>
@@ -5558,7 +5566,7 @@
         <v>64</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C81">
         <v>18</v>
@@ -5569,7 +5577,7 @@
         <v>65</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C82">
         <v>18</v>
@@ -5580,7 +5588,7 @@
         <v>67</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C83">
         <v>18</v>
@@ -5591,7 +5599,7 @@
         <v>69</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C84">
         <v>18</v>
@@ -5602,7 +5610,7 @@
         <v>70</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C85">
         <v>18</v>
@@ -5613,7 +5621,7 @@
         <v>71</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C86">
         <v>18</v>
@@ -5624,7 +5632,7 @@
         <v>73</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C87">
         <v>18</v>
@@ -5635,7 +5643,7 @@
         <v>75</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C88">
         <v>18</v>
@@ -5646,7 +5654,7 @@
         <v>76</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C89">
         <v>18</v>
@@ -5657,7 +5665,7 @@
         <v>77</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C90">
         <v>18</v>
@@ -5668,7 +5676,7 @@
         <v>78</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C91">
         <v>18</v>
@@ -5679,7 +5687,7 @@
         <v>80</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C92">
         <v>18</v>
@@ -5690,7 +5698,7 @@
         <v>81</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C93">
         <v>18</v>
@@ -5701,7 +5709,7 @@
         <v>83</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C94">
         <v>18</v>
@@ -5712,7 +5720,7 @@
         <v>84</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C95">
         <v>18</v>
@@ -5723,7 +5731,7 @@
         <v>86</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C96">
         <v>18</v>
@@ -5734,7 +5742,7 @@
         <v>87</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C97">
         <v>18</v>
@@ -5745,7 +5753,7 @@
         <v>88</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C98">
         <v>18</v>
@@ -5756,7 +5764,7 @@
         <v>90</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C99">
         <v>18</v>
@@ -5767,7 +5775,7 @@
         <v>92</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C100">
         <v>18</v>
@@ -5778,7 +5786,7 @@
         <v>93</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C101">
         <v>18</v>
@@ -5789,7 +5797,7 @@
         <v>94</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C102">
         <v>18</v>
@@ -5800,7 +5808,7 @@
         <v>96</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C103">
         <v>18</v>
@@ -5811,7 +5819,7 @@
         <v>97</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C104">
         <v>18</v>
@@ -5822,7 +5830,7 @@
         <v>98</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C105">
         <v>18</v>
@@ -5833,7 +5841,7 @@
         <v>100</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C106">
         <v>18</v>
@@ -5844,7 +5852,7 @@
         <v>101</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C107">
         <v>18</v>
@@ -5855,7 +5863,7 @@
         <v>103</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C108">
         <v>18</v>
@@ -5866,7 +5874,7 @@
         <v>105</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C109">
         <v>18</v>
@@ -5877,7 +5885,7 @@
         <v>106</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C110">
         <v>18</v>
@@ -5888,7 +5896,7 @@
         <v>109</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C111">
         <v>18</v>
@@ -5899,7 +5907,7 @@
         <v>110</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C112">
         <v>18</v>
@@ -5910,7 +5918,7 @@
         <v>111</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C113">
         <v>18</v>
@@ -5921,7 +5929,7 @@
         <v>112</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C114">
         <v>18</v>
@@ -5932,7 +5940,7 @@
         <v>113</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C115">
         <v>18</v>
@@ -5943,7 +5951,7 @@
         <v>114</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C116">
         <v>18</v>
@@ -5954,7 +5962,7 @@
         <v>115</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C117">
         <v>18</v>
@@ -5965,7 +5973,7 @@
         <v>116</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C118">
         <v>18</v>
@@ -5976,7 +5984,7 @@
         <v>117</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C119">
         <v>18</v>
@@ -5987,7 +5995,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C120">
         <v>18</v>
@@ -5998,7 +6006,7 @@
         <v>121</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C121">
         <v>18</v>
@@ -6009,7 +6017,7 @@
         <v>19</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C122">
         <v>21</v>
@@ -6020,7 +6028,7 @@
         <v>23</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C123">
         <v>21</v>
@@ -6031,7 +6039,7 @@
         <v>27</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C124">
         <v>21</v>
@@ -6042,7 +6050,7 @@
         <v>30</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C125">
         <v>21</v>
@@ -6053,7 +6061,7 @@
         <v>33</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C126">
         <v>21</v>
@@ -6064,7 +6072,7 @@
         <v>36</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C127">
         <v>21</v>
@@ -6075,7 +6083,7 @@
         <v>38</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C128">
         <v>21</v>
@@ -6086,7 +6094,7 @@
         <v>41</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C129">
         <v>21</v>
@@ -6097,7 +6105,7 @@
         <v>44</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C130">
         <v>21</v>
@@ -6108,7 +6116,7 @@
         <v>46</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C131">
         <v>21</v>
@@ -6119,7 +6127,7 @@
         <v>48</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C132">
         <v>21</v>
@@ -6130,7 +6138,7 @@
         <v>49</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C133">
         <v>21</v>
@@ -6141,7 +6149,7 @@
         <v>51</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C134">
         <v>21</v>
@@ -6152,7 +6160,7 @@
         <v>53</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C135">
         <v>21</v>
@@ -6163,7 +6171,7 @@
         <v>54</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C136">
         <v>21</v>
@@ -6174,7 +6182,7 @@
         <v>57</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C137">
         <v>21</v>
@@ -6185,7 +6193,7 @@
         <v>59</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C138">
         <v>21</v>
@@ -6196,7 +6204,7 @@
         <v>61</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C139">
         <v>21</v>
@@ -6207,7 +6215,7 @@
         <v>62</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C140">
         <v>21</v>
@@ -6218,7 +6226,7 @@
         <v>64</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C141">
         <v>21</v>
@@ -6229,7 +6237,7 @@
         <v>65</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C142">
         <v>21</v>
@@ -6240,7 +6248,7 @@
         <v>67</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C143">
         <v>21</v>
@@ -6251,7 +6259,7 @@
         <v>69</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C144">
         <v>21</v>
@@ -6262,7 +6270,7 @@
         <v>70</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C145">
         <v>21</v>
@@ -6273,7 +6281,7 @@
         <v>71</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C146">
         <v>21</v>
@@ -6284,7 +6292,7 @@
         <v>73</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C147">
         <v>21</v>
@@ -6295,7 +6303,7 @@
         <v>75</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C148">
         <v>21</v>
@@ -6306,7 +6314,7 @@
         <v>76</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C149">
         <v>21</v>
@@ -6317,7 +6325,7 @@
         <v>77</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C150">
         <v>21</v>
@@ -6328,7 +6336,7 @@
         <v>78</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C151">
         <v>21</v>
@@ -6339,7 +6347,7 @@
         <v>80</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C152">
         <v>21</v>
@@ -6350,7 +6358,7 @@
         <v>81</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C153">
         <v>21</v>
@@ -6361,7 +6369,7 @@
         <v>83</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C154">
         <v>21</v>
@@ -6372,7 +6380,7 @@
         <v>84</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C155">
         <v>21</v>
@@ -6383,7 +6391,7 @@
         <v>86</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C156">
         <v>21</v>
@@ -6394,7 +6402,7 @@
         <v>87</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C157">
         <v>21</v>
@@ -6405,7 +6413,7 @@
         <v>88</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C158">
         <v>21</v>
@@ -6416,7 +6424,7 @@
         <v>90</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C159">
         <v>21</v>
@@ -6427,7 +6435,7 @@
         <v>92</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C160">
         <v>21</v>
@@ -6438,7 +6446,7 @@
         <v>93</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C161">
         <v>21</v>
@@ -6449,7 +6457,7 @@
         <v>94</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C162">
         <v>21</v>
@@ -6460,7 +6468,7 @@
         <v>96</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C163">
         <v>21</v>
@@ -6471,7 +6479,7 @@
         <v>97</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C164">
         <v>21</v>
@@ -6482,7 +6490,7 @@
         <v>98</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C165">
         <v>21</v>
@@ -6493,7 +6501,7 @@
         <v>100</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C166">
         <v>21</v>
@@ -6504,7 +6512,7 @@
         <v>101</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C167">
         <v>21</v>
@@ -6515,7 +6523,7 @@
         <v>103</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C168">
         <v>21</v>
@@ -6526,7 +6534,7 @@
         <v>105</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C169">
         <v>21</v>
@@ -6537,7 +6545,7 @@
         <v>106</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C170">
         <v>21</v>
@@ -6548,7 +6556,7 @@
         <v>109</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C171">
         <v>21</v>
@@ -6559,7 +6567,7 @@
         <v>110</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C172">
         <v>21</v>
@@ -6570,7 +6578,7 @@
         <v>111</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C173">
         <v>21</v>
@@ -6581,7 +6589,7 @@
         <v>112</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C174">
         <v>21</v>
@@ -6592,7 +6600,7 @@
         <v>113</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C175">
         <v>21</v>
@@ -6603,7 +6611,7 @@
         <v>114</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C176">
         <v>21</v>
@@ -6614,7 +6622,7 @@
         <v>115</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C177">
         <v>21</v>
@@ -6625,7 +6633,7 @@
         <v>116</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C178">
         <v>21</v>
@@ -6636,7 +6644,7 @@
         <v>117</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C179">
         <v>21</v>
@@ -6647,7 +6655,7 @@
         <v>119</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C180">
         <v>21</v>
@@ -6658,7 +6666,7 @@
         <v>121</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C181">
         <v>21</v>
@@ -6669,7 +6677,7 @@
         <v>19</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C182">
         <v>10</v>
@@ -6680,7 +6688,7 @@
         <v>23</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C183">
         <v>10</v>
@@ -6691,7 +6699,7 @@
         <v>27</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C184">
         <v>10</v>
@@ -6702,7 +6710,7 @@
         <v>30</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C185">
         <v>10</v>
@@ -6713,7 +6721,7 @@
         <v>33</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C186">
         <v>10</v>
@@ -6724,7 +6732,7 @@
         <v>36</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C187">
         <v>10</v>
@@ -6735,7 +6743,7 @@
         <v>38</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C188">
         <v>10</v>
@@ -6746,7 +6754,7 @@
         <v>41</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C189">
         <v>10</v>
@@ -6757,7 +6765,7 @@
         <v>44</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C190">
         <v>10</v>
@@ -6768,7 +6776,7 @@
         <v>46</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C191">
         <v>10</v>
@@ -6779,7 +6787,7 @@
         <v>48</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C192">
         <v>10</v>
@@ -6790,7 +6798,7 @@
         <v>49</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C193">
         <v>10</v>
@@ -6801,7 +6809,7 @@
         <v>51</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C194">
         <v>10</v>
@@ -6812,7 +6820,7 @@
         <v>53</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C195">
         <v>10</v>
@@ -6823,7 +6831,7 @@
         <v>54</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C196">
         <v>10</v>
@@ -6834,7 +6842,7 @@
         <v>57</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C197">
         <v>10</v>
@@ -6845,7 +6853,7 @@
         <v>59</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C198">
         <v>10</v>
@@ -6856,7 +6864,7 @@
         <v>61</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C199">
         <v>10</v>
@@ -6867,7 +6875,7 @@
         <v>62</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C200">
         <v>10</v>
@@ -6878,7 +6886,7 @@
         <v>64</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C201">
         <v>10</v>
@@ -6889,7 +6897,7 @@
         <v>65</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C202">
         <v>10</v>
@@ -6900,7 +6908,7 @@
         <v>67</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C203">
         <v>10</v>
@@ -6911,7 +6919,7 @@
         <v>69</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C204">
         <v>10</v>
@@ -6922,7 +6930,7 @@
         <v>70</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C205">
         <v>10</v>
@@ -6933,7 +6941,7 @@
         <v>71</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C206">
         <v>10</v>
@@ -6944,7 +6952,7 @@
         <v>73</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C207">
         <v>10</v>
@@ -6955,7 +6963,7 @@
         <v>75</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C208">
         <v>10</v>
@@ -6966,7 +6974,7 @@
         <v>76</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C209">
         <v>10</v>
@@ -6977,7 +6985,7 @@
         <v>77</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C210">
         <v>10</v>
@@ -6988,7 +6996,7 @@
         <v>78</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C211">
         <v>10</v>
@@ -6999,7 +7007,7 @@
         <v>80</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C212">
         <v>10</v>
@@ -7010,7 +7018,7 @@
         <v>81</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C213">
         <v>10</v>
@@ -7021,7 +7029,7 @@
         <v>83</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C214">
         <v>10</v>
@@ -7032,7 +7040,7 @@
         <v>84</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C215">
         <v>10</v>
@@ -7043,7 +7051,7 @@
         <v>86</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C216">
         <v>10</v>
@@ -7054,7 +7062,7 @@
         <v>87</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C217">
         <v>10</v>
@@ -7065,7 +7073,7 @@
         <v>88</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C218">
         <v>10</v>
@@ -7076,7 +7084,7 @@
         <v>90</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C219">
         <v>10</v>
@@ -7087,7 +7095,7 @@
         <v>92</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C220">
         <v>10</v>
@@ -7098,7 +7106,7 @@
         <v>93</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C221">
         <v>10</v>
@@ -7109,7 +7117,7 @@
         <v>94</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C222">
         <v>10</v>
@@ -7120,7 +7128,7 @@
         <v>96</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C223">
         <v>10</v>
@@ -7131,7 +7139,7 @@
         <v>97</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C224">
         <v>10</v>
@@ -7142,7 +7150,7 @@
         <v>98</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C225">
         <v>10</v>
@@ -7153,7 +7161,7 @@
         <v>100</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C226">
         <v>10</v>
@@ -7164,7 +7172,7 @@
         <v>101</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C227">
         <v>10</v>
@@ -7175,7 +7183,7 @@
         <v>103</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C228">
         <v>10</v>
@@ -7186,7 +7194,7 @@
         <v>105</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C229">
         <v>10</v>
@@ -7197,7 +7205,7 @@
         <v>106</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C230">
         <v>10</v>
@@ -7208,7 +7216,7 @@
         <v>109</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C231">
         <v>10</v>
@@ -7219,7 +7227,7 @@
         <v>110</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C232">
         <v>10</v>
@@ -7230,7 +7238,7 @@
         <v>111</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C233">
         <v>10</v>
@@ -7241,7 +7249,7 @@
         <v>112</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C234">
         <v>10</v>
@@ -7252,7 +7260,7 @@
         <v>113</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C235">
         <v>10</v>
@@ -7263,7 +7271,7 @@
         <v>114</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C236">
         <v>10</v>
@@ -7274,7 +7282,7 @@
         <v>115</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C237">
         <v>10</v>
@@ -7285,7 +7293,7 @@
         <v>116</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C238">
         <v>10</v>
@@ -7296,7 +7304,7 @@
         <v>117</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C239">
         <v>10</v>
@@ -7307,7 +7315,7 @@
         <v>119</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C240">
         <v>10</v>
@@ -7318,7 +7326,7 @@
         <v>121</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C241">
         <v>10</v>
@@ -7345,7 +7353,7 @@
         <v>149</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -7353,7 +7361,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -7364,7 +7372,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -7375,7 +7383,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -7386,7 +7394,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -7397,7 +7405,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C6">
         <v>44</v>
@@ -7408,7 +7416,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C7">
         <v>44</v>
@@ -7419,7 +7427,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C8">
         <v>44</v>
@@ -7430,7 +7438,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C9">
         <v>44</v>

</xml_diff>

<commit_message>
changes on Dassault specs and template.
</commit_message>
<xml_diff>
--- a/data/template/official/template_in.xlsx
+++ b/data/template/official/template_in.xlsx
@@ -1,31 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pchtsp\Documents\projects\optima\data\template\official\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64751AC-F2A4-41F7-9B30-26A568685479}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0CB8EE-A811-46CD-9CE6-2513308B2DA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="623" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="623" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="maintenances" sheetId="1" r:id="rId1"/>
     <sheet name="etats_initiaux" sheetId="2" r:id="rId2"/>
     <sheet name="params" sheetId="3" r:id="rId3"/>
-    <sheet name="avions" sheetId="4" r:id="rId4"/>
-    <sheet name="heures_vol" sheetId="6" r:id="rId5"/>
-    <sheet name="maint_capacite" sheetId="7" r:id="rId6"/>
-    <sheet name="exemple_maints" sheetId="5" r:id="rId7"/>
+    <sheet name="missions" sheetId="8" r:id="rId4"/>
+    <sheet name="avions" sheetId="4" r:id="rId5"/>
+    <sheet name="heures_vol" sheetId="6" r:id="rId6"/>
+    <sheet name="maint_capacite" sheetId="7" r:id="rId7"/>
+    <sheet name="exemple_maints" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1298" uniqueCount="168">
   <si>
     <t>maint</t>
   </si>
@@ -521,6 +523,36 @@
   </si>
   <si>
     <t>2019-07</t>
+  </si>
+  <si>
+    <t>mission</t>
+  </si>
+  <si>
+    <t>nb_avions</t>
+  </si>
+  <si>
+    <t>type_avion</t>
+  </si>
+  <si>
+    <t>nb_heures</t>
+  </si>
+  <si>
+    <t>date_debut</t>
+  </si>
+  <si>
+    <t>date_fin</t>
+  </si>
+  <si>
+    <t>O1</t>
+  </si>
+  <si>
+    <t>2024-04</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>2022-04</t>
   </si>
 </sst>
 </file>
@@ -556,7 +588,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -579,16 +611,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3915,7 +3961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -3980,11 +4026,91 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1D2EB9-9068-4EFA-B083-EF0E14245526}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3994,7 +4120,7 @@
     <col min="4" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -4004,8 +4130,11 @@
       <c r="C1" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -4015,8 +4144,11 @@
       <c r="C2">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -4026,8 +4158,11 @@
       <c r="C3">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -4037,8 +4172,11 @@
       <c r="C4">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -4048,16 +4186,22 @@
       <c r="C5">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -4067,8 +4211,11 @@
       <c r="C7">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -4078,8 +4225,11 @@
       <c r="C8">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -4089,8 +4239,11 @@
       <c r="C9">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -4100,8 +4253,11 @@
       <c r="C10">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -4111,8 +4267,11 @@
       <c r="C11">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -4122,8 +4281,11 @@
       <c r="C12">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -4133,8 +4295,11 @@
       <c r="C13">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -4144,8 +4309,11 @@
       <c r="C14">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -4155,8 +4323,11 @@
       <c r="C15">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -4166,8 +4337,11 @@
       <c r="C16">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -4177,8 +4351,11 @@
       <c r="C17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>59</v>
       </c>
@@ -4188,8 +4365,11 @@
       <c r="C18">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -4199,8 +4379,11 @@
       <c r="C19">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -4210,8 +4393,11 @@
       <c r="C20">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>64</v>
       </c>
@@ -4221,8 +4407,11 @@
       <c r="C21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -4232,8 +4421,11 @@
       <c r="C22">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -4243,8 +4435,11 @@
       <c r="C23">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -4254,8 +4449,11 @@
       <c r="C24">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>70</v>
       </c>
@@ -4265,8 +4463,11 @@
       <c r="C25">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -4276,8 +4477,11 @@
       <c r="C26">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>73</v>
       </c>
@@ -4287,8 +4491,11 @@
       <c r="C27">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>75</v>
       </c>
@@ -4298,8 +4505,11 @@
       <c r="C28">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -4309,8 +4519,11 @@
       <c r="C29">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -4320,8 +4533,11 @@
       <c r="C30">
         <v>20</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>78</v>
       </c>
@@ -4331,8 +4547,11 @@
       <c r="C31">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>80</v>
       </c>
@@ -4342,8 +4561,11 @@
       <c r="C32">
         <v>20</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>81</v>
       </c>
@@ -4353,8 +4575,11 @@
       <c r="C33">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>83</v>
       </c>
@@ -4364,8 +4589,11 @@
       <c r="C34">
         <v>20</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -4375,8 +4603,11 @@
       <c r="C35">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>86</v>
       </c>
@@ -4386,8 +4617,11 @@
       <c r="C36">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>87</v>
       </c>
@@ -4397,8 +4631,11 @@
       <c r="C37">
         <v>20</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>88</v>
       </c>
@@ -4408,8 +4645,11 @@
       <c r="C38">
         <v>20</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>90</v>
       </c>
@@ -4419,8 +4659,11 @@
       <c r="C39">
         <v>20</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>92</v>
       </c>
@@ -4430,8 +4673,11 @@
       <c r="C40">
         <v>20</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>93</v>
       </c>
@@ -4441,8 +4687,11 @@
       <c r="C41">
         <v>20</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>94</v>
       </c>
@@ -4452,8 +4701,11 @@
       <c r="C42">
         <v>20</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>96</v>
       </c>
@@ -4463,8 +4715,11 @@
       <c r="C43">
         <v>20</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>97</v>
       </c>
@@ -4474,8 +4729,11 @@
       <c r="C44">
         <v>20</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>98</v>
       </c>
@@ -4485,8 +4743,11 @@
       <c r="C45">
         <v>20</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>100</v>
       </c>
@@ -4496,8 +4757,11 @@
       <c r="C46">
         <v>20</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>101</v>
       </c>
@@ -4507,8 +4771,11 @@
       <c r="C47">
         <v>20</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>103</v>
       </c>
@@ -4518,8 +4785,11 @@
       <c r="C48">
         <v>20</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>105</v>
       </c>
@@ -4529,8 +4799,11 @@
       <c r="C49">
         <v>20</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>106</v>
       </c>
@@ -4540,8 +4813,11 @@
       <c r="C50">
         <v>20</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>109</v>
       </c>
@@ -4551,8 +4827,11 @@
       <c r="C51">
         <v>20</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>110</v>
       </c>
@@ -4562,8 +4841,11 @@
       <c r="C52">
         <v>20</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>111</v>
       </c>
@@ -4573,8 +4855,11 @@
       <c r="C53">
         <v>20</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>112</v>
       </c>
@@ -4584,8 +4869,11 @@
       <c r="C54">
         <v>20</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>113</v>
       </c>
@@ -4595,8 +4883,11 @@
       <c r="C55">
         <v>20</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>114</v>
       </c>
@@ -4606,8 +4897,11 @@
       <c r="C56">
         <v>20</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>115</v>
       </c>
@@ -4617,8 +4911,11 @@
       <c r="C57">
         <v>20</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>116</v>
       </c>
@@ -4628,8 +4925,11 @@
       <c r="C58">
         <v>20</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>117</v>
       </c>
@@ -4639,8 +4939,11 @@
       <c r="C59">
         <v>20</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>119</v>
       </c>
@@ -4650,8 +4953,11 @@
       <c r="C60">
         <v>20</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>121</v>
       </c>
@@ -4660,6 +4966,9 @@
       </c>
       <c r="C61">
         <v>20</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4668,7 +4977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08E48A67-3B38-4D8C-86F5-29032CA09188}">
   <dimension ref="A1:C241"/>
   <sheetViews>
@@ -7337,7 +7646,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CA0ECB-0AB9-46DC-8B87-33A3FF49B522}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -7456,7 +7765,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
@@ -7658,19 +7967,19 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="288.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">

</xml_diff>